<commit_message>
Published state of ETDataset on 10 July 2015
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/coal.xlsx
+++ b/carriers_source_analyses/coal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="762" activeTab="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="99">
   <si>
     <t>Source</t>
   </si>
@@ -359,6 +359,9 @@
   <si>
     <t>Coal</t>
   </si>
+  <si>
+    <t>coal.yml</t>
+  </si>
 </sst>
 </file>
 
@@ -368,9 +371,9 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="171" formatCode="0.00000000"/>
-    <numFmt numFmtId="172" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="169" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1448,35 +1451,8 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1506,11 +1482,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="171" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="363">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2491,7 +2494,9 @@
       <c r="B5" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="122"/>
+      <c r="C5" s="122" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7"/>
@@ -2669,38 +2674,38 @@
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="136"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="158"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="137"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="139"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="161"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="140"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="142"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1">
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
     </row>
@@ -2797,7 +2802,7 @@
       <c r="F12" s="36"/>
       <c r="G12" s="113"/>
       <c r="H12" s="31"/>
-      <c r="I12" s="145"/>
+      <c r="I12" s="136"/>
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="2:11" s="44" customFormat="1" ht="19" thickBot="1">
@@ -2815,24 +2820,24 @@
       <c r="F13" s="36"/>
       <c r="G13" s="113"/>
       <c r="H13" s="31"/>
-      <c r="I13" s="145" t="s">
+      <c r="I13" s="136" t="s">
         <v>82</v>
       </c>
       <c r="J13" s="45"/>
     </row>
     <row r="14" spans="2:11" s="44" customFormat="1" ht="19" thickBot="1">
       <c r="B14" s="24"/>
-      <c r="C14" s="156" t="s">
+      <c r="C14" s="147" t="s">
         <v>86</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>87</v>
       </c>
       <c r="E14" s="115"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="156"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
       <c r="H14" s="31"/>
-      <c r="I14" s="145"/>
+      <c r="I14" s="136"/>
       <c r="J14" s="45"/>
     </row>
     <row r="15" spans="2:11" s="44" customFormat="1" ht="19" thickBot="1">
@@ -2850,7 +2855,7 @@
       <c r="F15" s="36"/>
       <c r="G15" s="113"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="145" t="s">
+      <c r="I15" s="136" t="s">
         <v>82</v>
       </c>
       <c r="J15" s="45"/>
@@ -2867,7 +2872,7 @@
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="145" t="s">
+      <c r="I16" s="136" t="s">
         <v>89</v>
       </c>
       <c r="J16" s="99"/>
@@ -2899,7 +2904,7 @@
     </row>
     <row r="19" spans="2:10" ht="16" thickBot="1">
       <c r="B19" s="40"/>
-      <c r="C19" s="156" t="s">
+      <c r="C19" s="147" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="113"/>
@@ -2918,7 +2923,7 @@
       <c r="D20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="163">
+      <c r="E20" s="154">
         <f>'Research data'!G15</f>
         <v>0</v>
       </c>
@@ -2940,7 +2945,7 @@
       <c r="D21" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="163">
+      <c r="E21" s="154">
         <f>'Research data'!G16</f>
         <v>3.12408E-3</v>
       </c>
@@ -2962,7 +2967,7 @@
       <c r="D22" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="163">
+      <c r="E22" s="154">
         <f>'Research data'!G17</f>
         <v>5.4969000000000003E-4</v>
       </c>
@@ -2984,7 +2989,7 @@
       <c r="D23" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="163">
+      <c r="E23" s="154">
         <f>'Research data'!G18</f>
         <v>3.3995999999999999E-4</v>
       </c>
@@ -3006,7 +3011,7 @@
       <c r="D24" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="163">
+      <c r="E24" s="154">
         <f>'Research data'!G19</f>
         <v>8.8163000000000005E-2</v>
       </c>
@@ -3028,7 +3033,7 @@
       <c r="D25" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="163">
+      <c r="E25" s="154">
         <f>'Research data'!G20</f>
         <v>0</v>
       </c>
@@ -3044,13 +3049,13 @@
     </row>
     <row r="26" spans="2:10" ht="16" thickBot="1">
       <c r="B26" s="40"/>
-      <c r="C26" s="158" t="s">
+      <c r="C26" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="143">
+      <c r="E26" s="134">
         <f>'Research data'!G21</f>
         <v>0.153</v>
       </c>
@@ -3064,22 +3069,22 @@
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="40"/>
-      <c r="C27" s="158"/>
+      <c r="C27" s="149"/>
       <c r="D27" s="23"/>
-      <c r="E27" s="164"/>
+      <c r="E27" s="155"/>
       <c r="F27" s="36"/>
       <c r="G27" s="113"/>
       <c r="H27" s="36"/>
-      <c r="I27" s="157"/>
+      <c r="I27" s="148"/>
       <c r="J27" s="99"/>
     </row>
     <row r="28" spans="2:10" ht="16" thickBot="1">
       <c r="B28" s="40"/>
-      <c r="C28" s="156" t="s">
+      <c r="C28" s="147" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="113"/>
-      <c r="E28" s="164"/>
+      <c r="E28" s="155"/>
       <c r="F28" s="113"/>
       <c r="G28" s="113"/>
       <c r="H28" s="113"/>
@@ -3094,7 +3099,7 @@
       <c r="D29" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="163">
+      <c r="E29" s="154">
         <f>'Research data'!G24</f>
         <v>0</v>
       </c>
@@ -3116,7 +3121,7 @@
       <c r="D30" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="163">
+      <c r="E30" s="154">
         <f>'Research data'!G25</f>
         <v>4.8553800000000003E-3</v>
       </c>
@@ -3138,7 +3143,7 @@
       <c r="D31" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="163">
+      <c r="E31" s="154">
         <f>'Research data'!G26</f>
         <v>1.26224E-3</v>
       </c>
@@ -3160,7 +3165,7 @@
       <c r="D32" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="163">
+      <c r="E32" s="154">
         <f>'Research data'!G27</f>
         <v>3.7334999999999999E-4</v>
       </c>
@@ -3182,7 +3187,7 @@
       <c r="D33" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="163">
+      <c r="E33" s="154">
         <f>'Research data'!G28</f>
         <v>9.8329299999999994E-2</v>
       </c>
@@ -3204,7 +3209,7 @@
       <c r="D34" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="163">
+      <c r="E34" s="154">
         <f>'Research data'!G29</f>
         <v>0</v>
       </c>
@@ -3220,13 +3225,13 @@
     </row>
     <row r="35" spans="2:10" ht="16" thickBot="1">
       <c r="B35" s="40"/>
-      <c r="C35" s="158" t="s">
+      <c r="C35" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="143">
+      <c r="E35" s="134">
         <f>'Research data'!G30</f>
         <v>0.124</v>
       </c>
@@ -3240,22 +3245,22 @@
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="40"/>
-      <c r="C36" s="158"/>
+      <c r="C36" s="149"/>
       <c r="D36" s="23"/>
-      <c r="E36" s="164"/>
+      <c r="E36" s="155"/>
       <c r="F36" s="36"/>
       <c r="G36" s="113"/>
       <c r="H36" s="36"/>
-      <c r="I36" s="157"/>
+      <c r="I36" s="148"/>
       <c r="J36" s="99"/>
     </row>
     <row r="37" spans="2:10" ht="16" thickBot="1">
       <c r="B37" s="40"/>
-      <c r="C37" s="156" t="s">
+      <c r="C37" s="147" t="s">
         <v>92</v>
       </c>
       <c r="D37" s="113"/>
-      <c r="E37" s="164"/>
+      <c r="E37" s="155"/>
       <c r="F37" s="113"/>
       <c r="G37" s="113"/>
       <c r="H37" s="113"/>
@@ -3270,7 +3275,7 @@
       <c r="D38" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="163">
+      <c r="E38" s="154">
         <f>'Research data'!G33</f>
         <v>0</v>
       </c>
@@ -3292,7 +3297,7 @@
       <c r="D39" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="163">
+      <c r="E39" s="154">
         <f>'Research data'!G34</f>
         <v>1.0756399999999999E-2</v>
       </c>
@@ -3314,7 +3319,7 @@
       <c r="D40" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="163">
+      <c r="E40" s="154">
         <f>'Research data'!G35</f>
         <v>1.5815200000000001E-3</v>
       </c>
@@ -3336,7 +3341,7 @@
       <c r="D41" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="163">
+      <c r="E41" s="154">
         <f>'Research data'!G36</f>
         <v>1.27921E-3</v>
       </c>
@@ -3358,7 +3363,7 @@
       <c r="D42" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E42" s="163">
+      <c r="E42" s="154">
         <f>'Research data'!G37</f>
         <v>0.103616</v>
       </c>
@@ -3380,7 +3385,7 @@
       <c r="D43" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="163">
+      <c r="E43" s="154">
         <f>'Research data'!G38</f>
         <v>0</v>
       </c>
@@ -3396,13 +3401,13 @@
     </row>
     <row r="44" spans="2:10" ht="16" thickBot="1">
       <c r="B44" s="40"/>
-      <c r="C44" s="158" t="s">
+      <c r="C44" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="143">
+      <c r="E44" s="134">
         <f>'Research data'!G39</f>
         <v>8.7999999999999995E-2</v>
       </c>
@@ -3416,22 +3421,22 @@
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="40"/>
-      <c r="C45" s="158"/>
+      <c r="C45" s="149"/>
       <c r="D45" s="23"/>
-      <c r="E45" s="164"/>
+      <c r="E45" s="155"/>
       <c r="F45" s="36"/>
       <c r="G45" s="113"/>
       <c r="H45" s="36"/>
-      <c r="I45" s="157"/>
+      <c r="I45" s="148"/>
       <c r="J45" s="99"/>
     </row>
     <row r="46" spans="2:10" ht="16" thickBot="1">
       <c r="B46" s="40"/>
-      <c r="C46" s="156" t="s">
+      <c r="C46" s="147" t="s">
         <v>93</v>
       </c>
       <c r="D46" s="113"/>
-      <c r="E46" s="164"/>
+      <c r="E46" s="155"/>
       <c r="F46" s="113"/>
       <c r="G46" s="113"/>
       <c r="H46" s="113"/>
@@ -3446,7 +3451,7 @@
       <c r="D47" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="163">
+      <c r="E47" s="154">
         <f>'Research data'!G42</f>
         <v>0</v>
       </c>
@@ -3468,7 +3473,7 @@
       <c r="D48" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="163">
+      <c r="E48" s="154">
         <f>'Research data'!G43</f>
         <v>3.6559299999999999E-3</v>
       </c>
@@ -3490,7 +3495,7 @@
       <c r="D49" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E49" s="163">
+      <c r="E49" s="154">
         <f>'Research data'!G44</f>
         <v>8.0710999999999999E-4</v>
       </c>
@@ -3512,7 +3517,7 @@
       <c r="D50" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="163">
+      <c r="E50" s="154">
         <f>'Research data'!G45</f>
         <v>2.1007E-4</v>
       </c>
@@ -3534,7 +3539,7 @@
       <c r="D51" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="163">
+      <c r="E51" s="154">
         <f>'Research data'!G46</f>
         <v>8.7446399999999994E-2</v>
       </c>
@@ -3556,7 +3561,7 @@
       <c r="D52" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="163">
+      <c r="E52" s="154">
         <f>'Research data'!G47</f>
         <v>0</v>
       </c>
@@ -3572,13 +3577,13 @@
     </row>
     <row r="53" spans="2:10" ht="16" thickBot="1">
       <c r="B53" s="40"/>
-      <c r="C53" s="158" t="s">
+      <c r="C53" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E53" s="143">
+      <c r="E53" s="134">
         <f>'Research data'!G48</f>
         <v>0.16900000000000001</v>
       </c>
@@ -3592,22 +3597,22 @@
     </row>
     <row r="54" spans="2:10">
       <c r="B54" s="40"/>
-      <c r="C54" s="158"/>
+      <c r="C54" s="149"/>
       <c r="D54" s="23"/>
-      <c r="E54" s="164"/>
+      <c r="E54" s="155"/>
       <c r="F54" s="36"/>
       <c r="G54" s="113"/>
       <c r="H54" s="36"/>
-      <c r="I54" s="157"/>
+      <c r="I54" s="148"/>
       <c r="J54" s="99"/>
     </row>
     <row r="55" spans="2:10" ht="16" thickBot="1">
       <c r="B55" s="40"/>
-      <c r="C55" s="156" t="s">
+      <c r="C55" s="147" t="s">
         <v>94</v>
       </c>
       <c r="D55" s="113"/>
-      <c r="E55" s="164"/>
+      <c r="E55" s="155"/>
       <c r="F55" s="113"/>
       <c r="G55" s="113"/>
       <c r="H55" s="113"/>
@@ -3622,7 +3627,7 @@
       <c r="D56" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="163">
+      <c r="E56" s="154">
         <f>'Research data'!G51</f>
         <v>0</v>
       </c>
@@ -3644,7 +3649,7 @@
       <c r="D57" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="163">
+      <c r="E57" s="154">
         <f>'Research data'!G52</f>
         <v>1.1964799999999999E-2</v>
       </c>
@@ -3666,7 +3671,7 @@
       <c r="D58" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E58" s="163">
+      <c r="E58" s="154">
         <f>'Research data'!G53</f>
         <v>2.0680500000000001E-3</v>
       </c>
@@ -3688,7 +3693,7 @@
       <c r="D59" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E59" s="163">
+      <c r="E59" s="154">
         <f>'Research data'!G54</f>
         <v>2.4298000000000001E-4</v>
       </c>
@@ -3710,7 +3715,7 @@
       <c r="D60" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E60" s="163">
+      <c r="E60" s="154">
         <f>'Research data'!G55</f>
         <v>9.9245600000000003E-2</v>
       </c>
@@ -3732,7 +3737,7 @@
       <c r="D61" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E61" s="163">
+      <c r="E61" s="154">
         <f>'Research data'!G56</f>
         <v>0</v>
       </c>
@@ -3748,13 +3753,13 @@
     </row>
     <row r="62" spans="2:10" ht="16" thickBot="1">
       <c r="B62" s="40"/>
-      <c r="C62" s="158" t="s">
+      <c r="C62" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D62" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E62" s="143">
+      <c r="E62" s="134">
         <f>'Research data'!G57</f>
         <v>0</v>
       </c>
@@ -3768,22 +3773,22 @@
     </row>
     <row r="63" spans="2:10">
       <c r="B63" s="40"/>
-      <c r="C63" s="158"/>
+      <c r="C63" s="149"/>
       <c r="D63" s="23"/>
-      <c r="E63" s="164"/>
+      <c r="E63" s="155"/>
       <c r="F63" s="36"/>
       <c r="G63" s="113"/>
       <c r="H63" s="36"/>
-      <c r="I63" s="157"/>
+      <c r="I63" s="148"/>
       <c r="J63" s="99"/>
     </row>
     <row r="64" spans="2:10" ht="16" thickBot="1">
       <c r="B64" s="40"/>
-      <c r="C64" s="156" t="s">
+      <c r="C64" s="147" t="s">
         <v>95</v>
       </c>
       <c r="D64" s="113"/>
-      <c r="E64" s="164"/>
+      <c r="E64" s="155"/>
       <c r="F64" s="113"/>
       <c r="G64" s="113"/>
       <c r="H64" s="113"/>
@@ -3798,7 +3803,7 @@
       <c r="D65" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E65" s="163">
+      <c r="E65" s="154">
         <f>'Research data'!G60</f>
         <v>0</v>
       </c>
@@ -3820,7 +3825,7 @@
       <c r="D66" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E66" s="163">
+      <c r="E66" s="154">
         <f>'Research data'!G61</f>
         <v>4.1242500000000003E-3</v>
       </c>
@@ -3842,7 +3847,7 @@
       <c r="D67" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E67" s="163">
+      <c r="E67" s="154">
         <f>'Research data'!G62</f>
         <v>5.9814999999999998E-4</v>
       </c>
@@ -3864,7 +3869,7 @@
       <c r="D68" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E68" s="163">
+      <c r="E68" s="154">
         <f>'Research data'!G63</f>
         <v>2.6328000000000001E-4</v>
       </c>
@@ -3886,7 +3891,7 @@
       <c r="D69" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E69" s="163">
+      <c r="E69" s="154">
         <f>'Research data'!G64</f>
         <v>9.0165499999999996E-2</v>
       </c>
@@ -3908,7 +3913,7 @@
       <c r="D70" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E70" s="163">
+      <c r="E70" s="154">
         <f>'Research data'!G65</f>
         <v>0</v>
       </c>
@@ -3924,13 +3929,13 @@
     </row>
     <row r="71" spans="2:10" ht="16" thickBot="1">
       <c r="B71" s="40"/>
-      <c r="C71" s="158" t="s">
+      <c r="C71" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D71" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="143">
+      <c r="E71" s="134">
         <f>'Research data'!G66</f>
         <v>0.26300000000000001</v>
       </c>
@@ -3944,22 +3949,22 @@
     </row>
     <row r="72" spans="2:10">
       <c r="B72" s="40"/>
-      <c r="C72" s="158"/>
+      <c r="C72" s="149"/>
       <c r="D72" s="23"/>
-      <c r="E72" s="164"/>
+      <c r="E72" s="155"/>
       <c r="F72" s="36"/>
       <c r="G72" s="113"/>
       <c r="H72" s="36"/>
-      <c r="I72" s="157"/>
+      <c r="I72" s="148"/>
       <c r="J72" s="99"/>
     </row>
     <row r="73" spans="2:10" ht="16" thickBot="1">
       <c r="B73" s="40"/>
-      <c r="C73" s="156" t="s">
+      <c r="C73" s="147" t="s">
         <v>96</v>
       </c>
       <c r="D73" s="113"/>
-      <c r="E73" s="164"/>
+      <c r="E73" s="155"/>
       <c r="F73" s="113"/>
       <c r="G73" s="113"/>
       <c r="H73" s="113"/>
@@ -3974,7 +3979,7 @@
       <c r="D74" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E74" s="163">
+      <c r="E74" s="154">
         <f>'Research data'!G69</f>
         <v>0</v>
       </c>
@@ -3996,7 +4001,7 @@
       <c r="D75" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E75" s="163">
+      <c r="E75" s="154">
         <f>'Research data'!G70</f>
         <v>5.1643000000000001E-4</v>
       </c>
@@ -4018,7 +4023,7 @@
       <c r="D76" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E76" s="163">
+      <c r="E76" s="154">
         <f>'Research data'!G71</f>
         <v>3.2445E-4</v>
       </c>
@@ -4040,7 +4045,7 @@
       <c r="D77" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E77" s="163">
+      <c r="E77" s="154">
         <f>'Research data'!G72</f>
         <v>2.8475000000000001E-4</v>
       </c>
@@ -4062,7 +4067,7 @@
       <c r="D78" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E78" s="163">
+      <c r="E78" s="154">
         <f>'Research data'!G73</f>
         <v>9.5493700000000001E-2</v>
       </c>
@@ -4084,7 +4089,7 @@
       <c r="D79" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E79" s="163">
+      <c r="E79" s="154">
         <f>'Research data'!G74</f>
         <v>0</v>
       </c>
@@ -4100,13 +4105,13 @@
     </row>
     <row r="80" spans="2:10" ht="16" thickBot="1">
       <c r="B80" s="40"/>
-      <c r="C80" s="158" t="s">
+      <c r="C80" s="149" t="s">
         <v>46</v>
       </c>
       <c r="D80" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E80" s="143">
+      <c r="E80" s="134">
         <f>'Research data'!G75</f>
         <v>0.20300000000000001</v>
       </c>
@@ -4120,13 +4125,13 @@
     </row>
     <row r="81" spans="2:10">
       <c r="B81" s="40"/>
-      <c r="C81" s="158"/>
+      <c r="C81" s="149"/>
       <c r="D81" s="23"/>
       <c r="E81" s="113"/>
       <c r="F81" s="36"/>
       <c r="G81" s="113"/>
       <c r="H81" s="36"/>
-      <c r="I81" s="157"/>
+      <c r="I81" s="148"/>
       <c r="J81" s="99"/>
     </row>
     <row r="82" spans="2:10" ht="20" customHeight="1" thickBot="1">
@@ -4347,25 +4352,25 @@
       <c r="N8" s="16"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="2:15" s="152" customFormat="1" ht="16" thickBot="1">
-      <c r="B9" s="148"/>
-      <c r="C9" s="149" t="s">
+    <row r="9" spans="2:15" s="143" customFormat="1" ht="16" thickBot="1">
+      <c r="B9" s="139"/>
+      <c r="C9" s="140" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="149"/>
-      <c r="E9" s="149"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140"/>
       <c r="F9" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="150"/>
-      <c r="H9" s="151"/>
-      <c r="I9" s="150"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="142"/>
+      <c r="I9" s="141"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="147"/>
+      <c r="O9" s="138"/>
     </row>
     <row r="10" spans="2:15" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B10" s="5"/>
@@ -4419,7 +4424,7 @@
       <c r="L11" s="18"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="147" t="s">
+      <c r="O11" s="138" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4455,7 +4460,7 @@
     </row>
     <row r="14" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B14" s="40"/>
-      <c r="C14" s="149" t="s">
+      <c r="C14" s="140" t="s">
         <v>90</v>
       </c>
       <c r="D14" s="113"/>
@@ -4475,14 +4480,14 @@
       <c r="F15" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="144">
+      <c r="G15" s="135">
         <f>K15</f>
         <v>0</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="35"/>
       <c r="J15" s="18"/>
-      <c r="K15" s="162">
+      <c r="K15" s="153">
         <f>Notes!H74</f>
         <v>0</v>
       </c>
@@ -4496,14 +4501,14 @@
       <c r="F16" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="144">
+      <c r="G16" s="135">
         <f t="shared" ref="G16:G21" si="0">K16</f>
         <v>3.12408E-3</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="35"/>
       <c r="J16" s="18"/>
-      <c r="K16" s="162">
+      <c r="K16" s="153">
         <f>Notes!H75</f>
         <v>3.12408E-3</v>
       </c>
@@ -4517,14 +4522,14 @@
       <c r="F17" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="144">
+      <c r="G17" s="135">
         <f t="shared" si="0"/>
         <v>5.4969000000000003E-4</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="35"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="162">
+      <c r="K17" s="153">
         <f>Notes!H76</f>
         <v>5.4969000000000003E-4</v>
       </c>
@@ -4538,14 +4543,14 @@
       <c r="F18" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="144">
+      <c r="G18" s="135">
         <f t="shared" si="0"/>
         <v>3.3995999999999999E-4</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="35"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="162">
+      <c r="K18" s="153">
         <f>Notes!H77</f>
         <v>3.3995999999999999E-4</v>
       </c>
@@ -4559,14 +4564,14 @@
       <c r="F19" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="144">
+      <c r="G19" s="135">
         <f t="shared" si="0"/>
         <v>8.8163000000000005E-2</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="35"/>
       <c r="J19" s="18"/>
-      <c r="K19" s="162">
+      <c r="K19" s="153">
         <f>Notes!H78</f>
         <v>8.8163000000000005E-2</v>
       </c>
@@ -4580,14 +4585,14 @@
       <c r="F20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="144">
+      <c r="G20" s="135">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="35"/>
       <c r="J20" s="18"/>
-      <c r="K20" s="162">
+      <c r="K20" s="153">
         <f>Notes!H79</f>
         <v>0</v>
       </c>
@@ -4595,20 +4600,20 @@
     </row>
     <row r="21" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B21" s="40"/>
-      <c r="C21" s="159" t="s">
+      <c r="C21" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="144">
+      <c r="G21" s="135">
         <f t="shared" si="0"/>
         <v>0.153</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="35"/>
       <c r="J21" s="18"/>
-      <c r="K21" s="161">
+      <c r="K21" s="152">
         <f>Notes!H80</f>
         <v>0.153</v>
       </c>
@@ -4616,18 +4621,18 @@
     </row>
     <row r="22" spans="2:15" s="37" customFormat="1">
       <c r="B22" s="40"/>
-      <c r="C22" s="159"/>
+      <c r="C22" s="150"/>
       <c r="F22" s="23"/>
       <c r="G22" s="113"/>
       <c r="H22" s="17"/>
       <c r="I22" s="35"/>
       <c r="J22" s="18"/>
-      <c r="K22" s="157"/>
+      <c r="K22" s="148"/>
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B23" s="40"/>
-      <c r="C23" s="149" t="s">
+      <c r="C23" s="140" t="s">
         <v>91</v>
       </c>
       <c r="F23" s="113"/>
@@ -4646,14 +4651,14 @@
       <c r="F24" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="144">
+      <c r="G24" s="135">
         <f>K24</f>
         <v>0</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="35"/>
       <c r="J24" s="18"/>
-      <c r="K24" s="162">
+      <c r="K24" s="153">
         <f>Notes!H83</f>
         <v>0</v>
       </c>
@@ -4667,14 +4672,14 @@
       <c r="F25" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="144">
+      <c r="G25" s="135">
         <f t="shared" ref="G25:G30" si="1">K25</f>
         <v>4.8553800000000003E-3</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="35"/>
       <c r="J25" s="18"/>
-      <c r="K25" s="162">
+      <c r="K25" s="153">
         <f>Notes!H84</f>
         <v>4.8553800000000003E-3</v>
       </c>
@@ -4688,14 +4693,14 @@
       <c r="F26" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="144">
+      <c r="G26" s="135">
         <f t="shared" si="1"/>
         <v>1.26224E-3</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="35"/>
       <c r="J26" s="18"/>
-      <c r="K26" s="162">
+      <c r="K26" s="153">
         <f>Notes!H85</f>
         <v>1.26224E-3</v>
       </c>
@@ -4709,14 +4714,14 @@
       <c r="F27" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="144">
+      <c r="G27" s="135">
         <f t="shared" si="1"/>
         <v>3.7334999999999999E-4</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="35"/>
       <c r="J27" s="18"/>
-      <c r="K27" s="162">
+      <c r="K27" s="153">
         <f>Notes!H86</f>
         <v>3.7334999999999999E-4</v>
       </c>
@@ -4730,14 +4735,14 @@
       <c r="F28" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="144">
+      <c r="G28" s="135">
         <f t="shared" si="1"/>
         <v>9.8329299999999994E-2</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="35"/>
       <c r="J28" s="18"/>
-      <c r="K28" s="162">
+      <c r="K28" s="153">
         <f>Notes!H87</f>
         <v>9.8329299999999994E-2</v>
       </c>
@@ -4751,14 +4756,14 @@
       <c r="F29" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="144">
+      <c r="G29" s="135">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="35"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="162">
+      <c r="K29" s="153">
         <f>Notes!H88</f>
         <v>0</v>
       </c>
@@ -4766,20 +4771,20 @@
     </row>
     <row r="30" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B30" s="40"/>
-      <c r="C30" s="159" t="s">
+      <c r="C30" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="144">
+      <c r="G30" s="135">
         <f t="shared" si="1"/>
         <v>0.124</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="35"/>
       <c r="J30" s="18"/>
-      <c r="K30" s="161">
+      <c r="K30" s="152">
         <f>Notes!H89</f>
         <v>0.124</v>
       </c>
@@ -4787,18 +4792,18 @@
     </row>
     <row r="31" spans="2:15" s="37" customFormat="1">
       <c r="B31" s="40"/>
-      <c r="C31" s="159"/>
+      <c r="C31" s="150"/>
       <c r="F31" s="23"/>
       <c r="G31" s="113"/>
       <c r="H31" s="17"/>
       <c r="I31" s="35"/>
       <c r="J31" s="18"/>
-      <c r="K31" s="157"/>
+      <c r="K31" s="148"/>
       <c r="O31" s="3"/>
     </row>
     <row r="32" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B32" s="40"/>
-      <c r="C32" s="149" t="s">
+      <c r="C32" s="140" t="s">
         <v>92</v>
       </c>
       <c r="F32" s="113"/>
@@ -4817,14 +4822,14 @@
       <c r="F33" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="144">
+      <c r="G33" s="135">
         <f>K33</f>
         <v>0</v>
       </c>
       <c r="H33" s="17"/>
       <c r="I33" s="35"/>
       <c r="J33" s="18"/>
-      <c r="K33" s="162">
+      <c r="K33" s="153">
         <f>Notes!H92</f>
         <v>0</v>
       </c>
@@ -4838,14 +4843,14 @@
       <c r="F34" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="144">
+      <c r="G34" s="135">
         <f t="shared" ref="G34:G39" si="2">K34</f>
         <v>1.0756399999999999E-2</v>
       </c>
       <c r="H34" s="17"/>
       <c r="I34" s="35"/>
       <c r="J34" s="18"/>
-      <c r="K34" s="162">
+      <c r="K34" s="153">
         <f>Notes!H93</f>
         <v>1.0756399999999999E-2</v>
       </c>
@@ -4859,14 +4864,14 @@
       <c r="F35" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="144">
+      <c r="G35" s="135">
         <f t="shared" si="2"/>
         <v>1.5815200000000001E-3</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="35"/>
       <c r="J35" s="18"/>
-      <c r="K35" s="162">
+      <c r="K35" s="153">
         <f>Notes!H94</f>
         <v>1.5815200000000001E-3</v>
       </c>
@@ -4880,14 +4885,14 @@
       <c r="F36" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G36" s="144">
+      <c r="G36" s="135">
         <f t="shared" si="2"/>
         <v>1.27921E-3</v>
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="35"/>
       <c r="J36" s="18"/>
-      <c r="K36" s="162">
+      <c r="K36" s="153">
         <f>Notes!H95</f>
         <v>1.27921E-3</v>
       </c>
@@ -4901,14 +4906,14 @@
       <c r="F37" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="144">
+      <c r="G37" s="135">
         <f t="shared" si="2"/>
         <v>0.103616</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="35"/>
       <c r="J37" s="18"/>
-      <c r="K37" s="162">
+      <c r="K37" s="153">
         <f>Notes!H96</f>
         <v>0.103616</v>
       </c>
@@ -4922,14 +4927,14 @@
       <c r="F38" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G38" s="144">
+      <c r="G38" s="135">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H38" s="17"/>
       <c r="I38" s="35"/>
       <c r="J38" s="18"/>
-      <c r="K38" s="162">
+      <c r="K38" s="153">
         <f>Notes!H97</f>
         <v>0</v>
       </c>
@@ -4937,20 +4942,20 @@
     </row>
     <row r="39" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B39" s="40"/>
-      <c r="C39" s="159" t="s">
+      <c r="C39" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="144">
+      <c r="G39" s="135">
         <f t="shared" si="2"/>
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="H39" s="17"/>
       <c r="I39" s="35"/>
       <c r="J39" s="18"/>
-      <c r="K39" s="161">
+      <c r="K39" s="152">
         <f>Notes!H98</f>
         <v>8.7999999999999995E-2</v>
       </c>
@@ -4958,18 +4963,18 @@
     </row>
     <row r="40" spans="2:15" s="37" customFormat="1">
       <c r="B40" s="40"/>
-      <c r="C40" s="159"/>
+      <c r="C40" s="150"/>
       <c r="F40" s="23"/>
       <c r="G40" s="113"/>
       <c r="H40" s="17"/>
       <c r="I40" s="35"/>
       <c r="J40" s="18"/>
-      <c r="K40" s="157"/>
+      <c r="K40" s="148"/>
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B41" s="40"/>
-      <c r="C41" s="149" t="s">
+      <c r="C41" s="140" t="s">
         <v>93</v>
       </c>
       <c r="F41" s="113"/>
@@ -4988,14 +4993,14 @@
       <c r="F42" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G42" s="144">
+      <c r="G42" s="135">
         <f>K42</f>
         <v>0</v>
       </c>
       <c r="H42" s="17"/>
       <c r="I42" s="35"/>
       <c r="J42" s="18"/>
-      <c r="K42" s="162">
+      <c r="K42" s="153">
         <f>Notes!H101</f>
         <v>0</v>
       </c>
@@ -5009,14 +5014,14 @@
       <c r="F43" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="144">
+      <c r="G43" s="135">
         <f t="shared" ref="G43:G48" si="3">K43</f>
         <v>3.6559299999999999E-3</v>
       </c>
       <c r="H43" s="17"/>
       <c r="I43" s="35"/>
       <c r="J43" s="18"/>
-      <c r="K43" s="162">
+      <c r="K43" s="153">
         <f>Notes!H102</f>
         <v>3.6559299999999999E-3</v>
       </c>
@@ -5030,14 +5035,14 @@
       <c r="F44" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="144">
+      <c r="G44" s="135">
         <f t="shared" si="3"/>
         <v>8.0710999999999999E-4</v>
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="35"/>
       <c r="J44" s="18"/>
-      <c r="K44" s="162">
+      <c r="K44" s="153">
         <f>Notes!H103</f>
         <v>8.0710999999999999E-4</v>
       </c>
@@ -5051,14 +5056,14 @@
       <c r="F45" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G45" s="144">
+      <c r="G45" s="135">
         <f t="shared" si="3"/>
         <v>2.1007E-4</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="35"/>
       <c r="J45" s="18"/>
-      <c r="K45" s="162">
+      <c r="K45" s="153">
         <f>Notes!H104</f>
         <v>2.1007E-4</v>
       </c>
@@ -5072,14 +5077,14 @@
       <c r="F46" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G46" s="144">
+      <c r="G46" s="135">
         <f t="shared" si="3"/>
         <v>8.7446399999999994E-2</v>
       </c>
       <c r="H46" s="17"/>
       <c r="I46" s="35"/>
       <c r="J46" s="18"/>
-      <c r="K46" s="162">
+      <c r="K46" s="153">
         <f>Notes!H105</f>
         <v>8.7446399999999994E-2</v>
       </c>
@@ -5093,14 +5098,14 @@
       <c r="F47" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G47" s="144">
+      <c r="G47" s="135">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="35"/>
       <c r="J47" s="18"/>
-      <c r="K47" s="162">
+      <c r="K47" s="153">
         <f>Notes!H106</f>
         <v>0</v>
       </c>
@@ -5108,20 +5113,20 @@
     </row>
     <row r="48" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B48" s="40"/>
-      <c r="C48" s="159" t="s">
+      <c r="C48" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F48" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G48" s="144">
+      <c r="G48" s="135">
         <f t="shared" si="3"/>
         <v>0.16900000000000001</v>
       </c>
       <c r="H48" s="17"/>
       <c r="I48" s="35"/>
       <c r="J48" s="18"/>
-      <c r="K48" s="161">
+      <c r="K48" s="152">
         <f>Notes!H107</f>
         <v>0.16900000000000001</v>
       </c>
@@ -5129,18 +5134,18 @@
     </row>
     <row r="49" spans="2:15" s="37" customFormat="1">
       <c r="B49" s="40"/>
-      <c r="C49" s="159"/>
+      <c r="C49" s="150"/>
       <c r="F49" s="23"/>
       <c r="G49" s="113"/>
       <c r="H49" s="17"/>
       <c r="I49" s="35"/>
       <c r="J49" s="18"/>
-      <c r="K49" s="157"/>
+      <c r="K49" s="148"/>
       <c r="O49" s="3"/>
     </row>
     <row r="50" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B50" s="40"/>
-      <c r="C50" s="149" t="s">
+      <c r="C50" s="140" t="s">
         <v>94</v>
       </c>
       <c r="F50" s="113"/>
@@ -5159,14 +5164,14 @@
       <c r="F51" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G51" s="144">
+      <c r="G51" s="135">
         <f>K51</f>
         <v>0</v>
       </c>
       <c r="H51" s="17"/>
       <c r="I51" s="35"/>
       <c r="J51" s="18"/>
-      <c r="K51" s="162">
+      <c r="K51" s="153">
         <f>Notes!H110</f>
         <v>0</v>
       </c>
@@ -5180,14 +5185,14 @@
       <c r="F52" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G52" s="144">
+      <c r="G52" s="135">
         <f t="shared" ref="G52:G57" si="4">K52</f>
         <v>1.1964799999999999E-2</v>
       </c>
       <c r="H52" s="17"/>
       <c r="I52" s="35"/>
       <c r="J52" s="18"/>
-      <c r="K52" s="162">
+      <c r="K52" s="153">
         <f>Notes!H111</f>
         <v>1.1964799999999999E-2</v>
       </c>
@@ -5201,14 +5206,14 @@
       <c r="F53" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G53" s="144">
+      <c r="G53" s="135">
         <f t="shared" si="4"/>
         <v>2.0680500000000001E-3</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="35"/>
       <c r="J53" s="18"/>
-      <c r="K53" s="162">
+      <c r="K53" s="153">
         <f>Notes!H112</f>
         <v>2.0680500000000001E-3</v>
       </c>
@@ -5222,14 +5227,14 @@
       <c r="F54" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G54" s="144">
+      <c r="G54" s="135">
         <f t="shared" si="4"/>
         <v>2.4298000000000001E-4</v>
       </c>
       <c r="H54" s="17"/>
       <c r="I54" s="35"/>
       <c r="J54" s="18"/>
-      <c r="K54" s="162">
+      <c r="K54" s="153">
         <f>Notes!H113</f>
         <v>2.4298000000000001E-4</v>
       </c>
@@ -5243,14 +5248,14 @@
       <c r="F55" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G55" s="144">
+      <c r="G55" s="135">
         <f t="shared" si="4"/>
         <v>9.9245600000000003E-2</v>
       </c>
       <c r="H55" s="17"/>
       <c r="I55" s="35"/>
       <c r="J55" s="18"/>
-      <c r="K55" s="162">
+      <c r="K55" s="153">
         <f>Notes!H114</f>
         <v>9.9245600000000003E-2</v>
       </c>
@@ -5264,14 +5269,14 @@
       <c r="F56" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G56" s="144">
+      <c r="G56" s="135">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H56" s="17"/>
       <c r="I56" s="35"/>
       <c r="J56" s="18"/>
-      <c r="K56" s="162">
+      <c r="K56" s="153">
         <f>Notes!H115</f>
         <v>0</v>
       </c>
@@ -5279,20 +5284,20 @@
     </row>
     <row r="57" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B57" s="40"/>
-      <c r="C57" s="159" t="s">
+      <c r="C57" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F57" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G57" s="144">
+      <c r="G57" s="135">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H57" s="17"/>
       <c r="I57" s="35"/>
       <c r="J57" s="18"/>
-      <c r="K57" s="161">
+      <c r="K57" s="152">
         <f>Notes!H116</f>
         <v>0</v>
       </c>
@@ -5300,18 +5305,18 @@
     </row>
     <row r="58" spans="2:15" s="37" customFormat="1">
       <c r="B58" s="40"/>
-      <c r="C58" s="159"/>
+      <c r="C58" s="150"/>
       <c r="F58" s="23"/>
       <c r="G58" s="113"/>
       <c r="H58" s="17"/>
       <c r="I58" s="35"/>
       <c r="J58" s="18"/>
-      <c r="K58" s="157"/>
+      <c r="K58" s="148"/>
       <c r="O58" s="3"/>
     </row>
     <row r="59" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B59" s="40"/>
-      <c r="C59" s="149" t="s">
+      <c r="C59" s="140" t="s">
         <v>95</v>
       </c>
       <c r="F59" s="113"/>
@@ -5330,14 +5335,14 @@
       <c r="F60" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G60" s="144">
+      <c r="G60" s="135">
         <f>K60</f>
         <v>0</v>
       </c>
       <c r="H60" s="17"/>
       <c r="I60" s="35"/>
       <c r="J60" s="18"/>
-      <c r="K60" s="162">
+      <c r="K60" s="153">
         <f>Notes!H119</f>
         <v>0</v>
       </c>
@@ -5351,14 +5356,14 @@
       <c r="F61" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G61" s="144">
+      <c r="G61" s="135">
         <f t="shared" ref="G61:G66" si="5">K61</f>
         <v>4.1242500000000003E-3</v>
       </c>
       <c r="H61" s="17"/>
       <c r="I61" s="35"/>
       <c r="J61" s="18"/>
-      <c r="K61" s="162">
+      <c r="K61" s="153">
         <f>Notes!H120</f>
         <v>4.1242500000000003E-3</v>
       </c>
@@ -5372,14 +5377,14 @@
       <c r="F62" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G62" s="144">
+      <c r="G62" s="135">
         <f t="shared" si="5"/>
         <v>5.9814999999999998E-4</v>
       </c>
       <c r="H62" s="17"/>
       <c r="I62" s="35"/>
       <c r="J62" s="18"/>
-      <c r="K62" s="162">
+      <c r="K62" s="153">
         <f>Notes!H121</f>
         <v>5.9814999999999998E-4</v>
       </c>
@@ -5393,14 +5398,14 @@
       <c r="F63" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G63" s="144">
+      <c r="G63" s="135">
         <f t="shared" si="5"/>
         <v>2.6328000000000001E-4</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="35"/>
       <c r="J63" s="18"/>
-      <c r="K63" s="162">
+      <c r="K63" s="153">
         <f>Notes!H122</f>
         <v>2.6328000000000001E-4</v>
       </c>
@@ -5414,14 +5419,14 @@
       <c r="F64" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G64" s="144">
+      <c r="G64" s="135">
         <f t="shared" si="5"/>
         <v>9.0165499999999996E-2</v>
       </c>
       <c r="H64" s="17"/>
       <c r="I64" s="35"/>
       <c r="J64" s="18"/>
-      <c r="K64" s="162">
+      <c r="K64" s="153">
         <f>Notes!H123</f>
         <v>9.0165499999999996E-2</v>
       </c>
@@ -5435,14 +5440,14 @@
       <c r="F65" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G65" s="144">
+      <c r="G65" s="135">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H65" s="17"/>
       <c r="I65" s="35"/>
       <c r="J65" s="18"/>
-      <c r="K65" s="162">
+      <c r="K65" s="153">
         <f>Notes!H124</f>
         <v>0</v>
       </c>
@@ -5450,20 +5455,20 @@
     </row>
     <row r="66" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B66" s="40"/>
-      <c r="C66" s="159" t="s">
+      <c r="C66" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F66" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G66" s="144">
+      <c r="G66" s="135">
         <f t="shared" si="5"/>
         <v>0.26300000000000001</v>
       </c>
       <c r="H66" s="17"/>
       <c r="I66" s="35"/>
       <c r="J66" s="18"/>
-      <c r="K66" s="161">
+      <c r="K66" s="152">
         <f>Notes!H125</f>
         <v>0.26300000000000001</v>
       </c>
@@ -5471,18 +5476,18 @@
     </row>
     <row r="67" spans="2:15" s="37" customFormat="1">
       <c r="B67" s="40"/>
-      <c r="C67" s="159"/>
+      <c r="C67" s="150"/>
       <c r="F67" s="23"/>
       <c r="G67" s="113"/>
       <c r="H67" s="17"/>
       <c r="I67" s="35"/>
       <c r="J67" s="18"/>
-      <c r="K67" s="157"/>
+      <c r="K67" s="148"/>
       <c r="O67" s="3"/>
     </row>
     <row r="68" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B68" s="40"/>
-      <c r="C68" s="149" t="s">
+      <c r="C68" s="140" t="s">
         <v>96</v>
       </c>
       <c r="F68" s="113"/>
@@ -5501,14 +5506,14 @@
       <c r="F69" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G69" s="144">
+      <c r="G69" s="135">
         <f>K69</f>
         <v>0</v>
       </c>
       <c r="H69" s="17"/>
       <c r="I69" s="35"/>
       <c r="J69" s="18"/>
-      <c r="K69" s="162">
+      <c r="K69" s="153">
         <f>Notes!H128</f>
         <v>0</v>
       </c>
@@ -5522,14 +5527,14 @@
       <c r="F70" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G70" s="144">
+      <c r="G70" s="135">
         <f t="shared" ref="G70:G75" si="6">K70</f>
         <v>5.1643000000000001E-4</v>
       </c>
       <c r="H70" s="17"/>
       <c r="I70" s="35"/>
       <c r="J70" s="18"/>
-      <c r="K70" s="162">
+      <c r="K70" s="153">
         <f>Notes!H129</f>
         <v>5.1643000000000001E-4</v>
       </c>
@@ -5543,14 +5548,14 @@
       <c r="F71" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G71" s="144">
+      <c r="G71" s="135">
         <f t="shared" si="6"/>
         <v>3.2445E-4</v>
       </c>
       <c r="H71" s="17"/>
       <c r="I71" s="35"/>
       <c r="J71" s="18"/>
-      <c r="K71" s="162">
+      <c r="K71" s="153">
         <f>Notes!H130</f>
         <v>3.2445E-4</v>
       </c>
@@ -5564,14 +5569,14 @@
       <c r="F72" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G72" s="144">
+      <c r="G72" s="135">
         <f t="shared" si="6"/>
         <v>2.8475000000000001E-4</v>
       </c>
       <c r="H72" s="17"/>
       <c r="I72" s="35"/>
       <c r="J72" s="18"/>
-      <c r="K72" s="162">
+      <c r="K72" s="153">
         <f>Notes!H131</f>
         <v>2.8475000000000001E-4</v>
       </c>
@@ -5585,14 +5590,14 @@
       <c r="F73" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G73" s="144">
+      <c r="G73" s="135">
         <f t="shared" si="6"/>
         <v>9.5493700000000001E-2</v>
       </c>
       <c r="H73" s="17"/>
       <c r="I73" s="35"/>
       <c r="J73" s="18"/>
-      <c r="K73" s="162">
+      <c r="K73" s="153">
         <f>Notes!H132</f>
         <v>9.5493700000000001E-2</v>
       </c>
@@ -5606,14 +5611,14 @@
       <c r="F74" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G74" s="144">
+      <c r="G74" s="135">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H74" s="17"/>
       <c r="I74" s="35"/>
       <c r="J74" s="18"/>
-      <c r="K74" s="162">
+      <c r="K74" s="153">
         <f>Notes!H133</f>
         <v>0</v>
       </c>
@@ -5621,20 +5626,20 @@
     </row>
     <row r="75" spans="2:15" s="37" customFormat="1" ht="16" thickBot="1">
       <c r="B75" s="40"/>
-      <c r="C75" s="159" t="s">
+      <c r="C75" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F75" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G75" s="144">
+      <c r="G75" s="135">
         <f t="shared" si="6"/>
         <v>0.20300000000000001</v>
       </c>
       <c r="H75" s="17"/>
       <c r="I75" s="35"/>
       <c r="J75" s="18"/>
-      <c r="K75" s="161">
+      <c r="K75" s="152">
         <f>Notes!H134</f>
         <v>0.20300000000000001</v>
       </c>
@@ -5642,13 +5647,13 @@
     </row>
     <row r="76" spans="2:15" s="37" customFormat="1">
       <c r="B76" s="40"/>
-      <c r="C76" s="158"/>
+      <c r="C76" s="149"/>
       <c r="D76" s="23"/>
       <c r="E76" s="113"/>
       <c r="F76" s="36"/>
       <c r="G76" s="113"/>
       <c r="H76" s="17"/>
-      <c r="I76" s="157"/>
+      <c r="I76" s="148"/>
       <c r="J76" s="18"/>
       <c r="O76" s="3"/>
     </row>
@@ -5931,14 +5936,14 @@
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="53"/>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="144" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="61"/>
-      <c r="E7" s="146" t="s">
+      <c r="E7" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="146" t="s">
+      <c r="F7" s="137" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="56" t="s">
@@ -5958,7 +5963,7 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="53"/>
-      <c r="C8" s="154" t="s">
+      <c r="C8" s="145" t="s">
         <v>86</v>
       </c>
       <c r="E8" s="131"/>
@@ -5966,7 +5971,7 @@
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="53"/>
-      <c r="C9" s="155" t="s">
+      <c r="C9" s="146" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="131"/>
@@ -7037,7 +7042,7 @@
       </c>
     </row>
     <row r="73" spans="2:25">
-      <c r="E73" s="149" t="s">
+      <c r="E73" s="140" t="s">
         <v>90</v>
       </c>
       <c r="F73" s="113"/>
@@ -7050,7 +7055,7 @@
       </c>
       <c r="F74" s="37"/>
       <c r="G74" s="37"/>
-      <c r="H74" s="160">
+      <c r="H74" s="151">
         <v>0</v>
       </c>
       <c r="I74" s="123" t="s">
@@ -7067,7 +7072,7 @@
       </c>
       <c r="F75" s="37"/>
       <c r="G75" s="37"/>
-      <c r="H75" s="160">
+      <c r="H75" s="151">
         <v>3.12408E-3</v>
       </c>
       <c r="I75" s="123" t="s">
@@ -7082,7 +7087,7 @@
       </c>
       <c r="F76" s="37"/>
       <c r="G76" s="37"/>
-      <c r="H76" s="160">
+      <c r="H76" s="151">
         <v>5.4969000000000003E-4</v>
       </c>
       <c r="I76" s="123" t="s">
@@ -7098,7 +7103,7 @@
       </c>
       <c r="F77" s="37"/>
       <c r="G77" s="37"/>
-      <c r="H77" s="160">
+      <c r="H77" s="151">
         <v>3.3995999999999999E-4</v>
       </c>
       <c r="I77" s="123" t="s">
@@ -7114,7 +7119,7 @@
       </c>
       <c r="F78" s="37"/>
       <c r="G78" s="37"/>
-      <c r="H78" s="160">
+      <c r="H78" s="151">
         <v>8.8163000000000005E-2</v>
       </c>
       <c r="I78" s="123" t="s">
@@ -7130,7 +7135,7 @@
       </c>
       <c r="F79" s="37"/>
       <c r="G79" s="37"/>
-      <c r="H79" s="160">
+      <c r="H79" s="151">
         <v>0</v>
       </c>
       <c r="I79" s="123" t="s">
@@ -7143,7 +7148,7 @@
     </row>
     <row r="80" spans="2:25">
       <c r="D80" s="123"/>
-      <c r="E80" s="159" t="s">
+      <c r="E80" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F80" s="37"/>
@@ -7158,7 +7163,7 @@
     </row>
     <row r="81" spans="4:11">
       <c r="D81" s="123"/>
-      <c r="E81" s="159"/>
+      <c r="E81" s="150"/>
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
       <c r="H81" s="23"/>
@@ -7167,7 +7172,7 @@
     </row>
     <row r="82" spans="4:11">
       <c r="D82" s="123"/>
-      <c r="E82" s="149" t="s">
+      <c r="E82" s="140" t="s">
         <v>91</v>
       </c>
       <c r="F82" s="37"/>
@@ -7184,7 +7189,7 @@
       </c>
       <c r="F83" s="37"/>
       <c r="G83" s="37"/>
-      <c r="H83" s="160">
+      <c r="H83" s="151">
         <v>0</v>
       </c>
       <c r="I83" s="123" t="s">
@@ -7199,7 +7204,7 @@
       </c>
       <c r="F84" s="37"/>
       <c r="G84" s="37"/>
-      <c r="H84" s="160">
+      <c r="H84" s="151">
         <v>4.8553800000000003E-3</v>
       </c>
       <c r="I84" s="123" t="s">
@@ -7214,7 +7219,7 @@
       </c>
       <c r="F85" s="37"/>
       <c r="G85" s="37"/>
-      <c r="H85" s="160">
+      <c r="H85" s="151">
         <v>1.26224E-3</v>
       </c>
       <c r="I85" s="123" t="s">
@@ -7229,7 +7234,7 @@
       </c>
       <c r="F86" s="37"/>
       <c r="G86" s="37"/>
-      <c r="H86" s="160">
+      <c r="H86" s="151">
         <v>3.7334999999999999E-4</v>
       </c>
       <c r="I86" s="123" t="s">
@@ -7244,7 +7249,7 @@
       </c>
       <c r="F87" s="37"/>
       <c r="G87" s="37"/>
-      <c r="H87" s="160">
+      <c r="H87" s="151">
         <v>9.8329299999999994E-2</v>
       </c>
       <c r="I87" s="123" t="s">
@@ -7261,7 +7266,7 @@
       </c>
       <c r="F88" s="37"/>
       <c r="G88" s="37"/>
-      <c r="H88" s="160">
+      <c r="H88" s="151">
         <v>0</v>
       </c>
       <c r="I88" s="123" t="s">
@@ -7269,7 +7274,7 @@
       </c>
     </row>
     <row r="89" spans="4:11">
-      <c r="E89" s="159" t="s">
+      <c r="E89" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F89" s="37"/>
@@ -7282,7 +7287,7 @@
       </c>
     </row>
     <row r="90" spans="4:11">
-      <c r="E90" s="159"/>
+      <c r="E90" s="150"/>
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
       <c r="H90" s="23"/>
@@ -7291,7 +7296,7 @@
       <c r="K90" s="133"/>
     </row>
     <row r="91" spans="4:11">
-      <c r="E91" s="149" t="s">
+      <c r="E91" s="140" t="s">
         <v>92</v>
       </c>
       <c r="F91" s="37"/>
@@ -7306,7 +7311,7 @@
       </c>
       <c r="F92" s="37"/>
       <c r="G92" s="37"/>
-      <c r="H92" s="160">
+      <c r="H92" s="151">
         <v>0</v>
       </c>
       <c r="I92" s="123" t="s">
@@ -7321,7 +7326,7 @@
       </c>
       <c r="F93" s="37"/>
       <c r="G93" s="37"/>
-      <c r="H93" s="160">
+      <c r="H93" s="151">
         <v>1.0756399999999999E-2</v>
       </c>
       <c r="I93" s="123" t="s">
@@ -7336,7 +7341,7 @@
       </c>
       <c r="F94" s="37"/>
       <c r="G94" s="37"/>
-      <c r="H94" s="160">
+      <c r="H94" s="151">
         <v>1.5815200000000001E-3</v>
       </c>
       <c r="I94" s="123" t="s">
@@ -7351,7 +7356,7 @@
       </c>
       <c r="F95" s="37"/>
       <c r="G95" s="37"/>
-      <c r="H95" s="160">
+      <c r="H95" s="151">
         <v>1.27921E-3</v>
       </c>
       <c r="I95" s="123" t="s">
@@ -7366,7 +7371,7 @@
       </c>
       <c r="F96" s="37"/>
       <c r="G96" s="37"/>
-      <c r="H96" s="160">
+      <c r="H96" s="151">
         <v>0.103616</v>
       </c>
       <c r="I96" s="123" t="s">
@@ -7381,7 +7386,7 @@
       </c>
       <c r="F97" s="37"/>
       <c r="G97" s="37"/>
-      <c r="H97" s="160">
+      <c r="H97" s="151">
         <v>0</v>
       </c>
       <c r="I97" s="123" t="s">
@@ -7391,7 +7396,7 @@
       <c r="K97" s="133"/>
     </row>
     <row r="98" spans="5:11">
-      <c r="E98" s="159" t="s">
+      <c r="E98" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F98" s="37"/>
@@ -7406,7 +7411,7 @@
       <c r="K98" s="133"/>
     </row>
     <row r="99" spans="5:11">
-      <c r="E99" s="159"/>
+      <c r="E99" s="150"/>
       <c r="F99" s="37"/>
       <c r="G99" s="37"/>
       <c r="H99" s="23"/>
@@ -7415,7 +7420,7 @@
       <c r="K99" s="123"/>
     </row>
     <row r="100" spans="5:11">
-      <c r="E100" s="149" t="s">
+      <c r="E100" s="140" t="s">
         <v>93</v>
       </c>
       <c r="F100" s="37"/>
@@ -7430,7 +7435,7 @@
       </c>
       <c r="F101" s="37"/>
       <c r="G101" s="37"/>
-      <c r="H101" s="160">
+      <c r="H101" s="151">
         <v>0</v>
       </c>
       <c r="I101" s="123" t="s">
@@ -7445,7 +7450,7 @@
       </c>
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
-      <c r="H102" s="160">
+      <c r="H102" s="151">
         <v>3.6559299999999999E-3</v>
       </c>
       <c r="I102" s="123" t="s">
@@ -7460,7 +7465,7 @@
       </c>
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
-      <c r="H103" s="160">
+      <c r="H103" s="151">
         <v>8.0710999999999999E-4</v>
       </c>
       <c r="I103" s="123" t="s">
@@ -7475,7 +7480,7 @@
       </c>
       <c r="F104" s="37"/>
       <c r="G104" s="37"/>
-      <c r="H104" s="160">
+      <c r="H104" s="151">
         <v>2.1007E-4</v>
       </c>
       <c r="I104" s="123" t="s">
@@ -7490,7 +7495,7 @@
       </c>
       <c r="F105" s="37"/>
       <c r="G105" s="37"/>
-      <c r="H105" s="160">
+      <c r="H105" s="151">
         <v>8.7446399999999994E-2</v>
       </c>
       <c r="I105" s="123" t="s">
@@ -7503,7 +7508,7 @@
       </c>
       <c r="F106" s="37"/>
       <c r="G106" s="37"/>
-      <c r="H106" s="160">
+      <c r="H106" s="151">
         <v>0</v>
       </c>
       <c r="I106" s="123" t="s">
@@ -7511,7 +7516,7 @@
       </c>
     </row>
     <row r="107" spans="5:11">
-      <c r="E107" s="159" t="s">
+      <c r="E107" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F107" s="37"/>
@@ -7524,13 +7529,13 @@
       </c>
     </row>
     <row r="108" spans="5:11">
-      <c r="E108" s="159"/>
+      <c r="E108" s="150"/>
       <c r="F108" s="37"/>
       <c r="G108" s="37"/>
       <c r="H108" s="23"/>
     </row>
     <row r="109" spans="5:11">
-      <c r="E109" s="149" t="s">
+      <c r="E109" s="140" t="s">
         <v>94</v>
       </c>
       <c r="F109" s="37"/>
@@ -7543,7 +7548,7 @@
       </c>
       <c r="F110" s="37"/>
       <c r="G110" s="37"/>
-      <c r="H110" s="160">
+      <c r="H110" s="151">
         <v>0</v>
       </c>
       <c r="I110" s="123" t="s">
@@ -7556,7 +7561,7 @@
       </c>
       <c r="F111" s="37"/>
       <c r="G111" s="37"/>
-      <c r="H111" s="160">
+      <c r="H111" s="151">
         <v>1.1964799999999999E-2</v>
       </c>
       <c r="I111" s="123" t="s">
@@ -7569,7 +7574,7 @@
       </c>
       <c r="F112" s="37"/>
       <c r="G112" s="37"/>
-      <c r="H112" s="160">
+      <c r="H112" s="151">
         <v>2.0680500000000001E-3</v>
       </c>
       <c r="I112" s="123" t="s">
@@ -7582,7 +7587,7 @@
       </c>
       <c r="F113" s="37"/>
       <c r="G113" s="37"/>
-      <c r="H113" s="160">
+      <c r="H113" s="151">
         <v>2.4298000000000001E-4</v>
       </c>
       <c r="I113" s="123" t="s">
@@ -7595,7 +7600,7 @@
       </c>
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
-      <c r="H114" s="160">
+      <c r="H114" s="151">
         <v>9.9245600000000003E-2</v>
       </c>
       <c r="I114" s="123" t="s">
@@ -7608,7 +7613,7 @@
       </c>
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
-      <c r="H115" s="160">
+      <c r="H115" s="151">
         <v>0</v>
       </c>
       <c r="I115" s="123" t="s">
@@ -7616,7 +7621,7 @@
       </c>
     </row>
     <row r="116" spans="5:9">
-      <c r="E116" s="159" t="s">
+      <c r="E116" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F116" s="37"/>
@@ -7629,13 +7634,13 @@
       </c>
     </row>
     <row r="117" spans="5:9">
-      <c r="E117" s="159"/>
+      <c r="E117" s="150"/>
       <c r="F117" s="37"/>
       <c r="G117" s="37"/>
       <c r="H117" s="23"/>
     </row>
     <row r="118" spans="5:9">
-      <c r="E118" s="149" t="s">
+      <c r="E118" s="140" t="s">
         <v>95</v>
       </c>
       <c r="F118" s="37"/>
@@ -7648,7 +7653,7 @@
       </c>
       <c r="F119" s="37"/>
       <c r="G119" s="37"/>
-      <c r="H119" s="160">
+      <c r="H119" s="151">
         <v>0</v>
       </c>
       <c r="I119" s="123" t="s">
@@ -7661,7 +7666,7 @@
       </c>
       <c r="F120" s="37"/>
       <c r="G120" s="37"/>
-      <c r="H120" s="160">
+      <c r="H120" s="151">
         <v>4.1242500000000003E-3</v>
       </c>
       <c r="I120" s="123" t="s">
@@ -7674,7 +7679,7 @@
       </c>
       <c r="F121" s="37"/>
       <c r="G121" s="37"/>
-      <c r="H121" s="160">
+      <c r="H121" s="151">
         <v>5.9814999999999998E-4</v>
       </c>
       <c r="I121" s="123" t="s">
@@ -7687,7 +7692,7 @@
       </c>
       <c r="F122" s="37"/>
       <c r="G122" s="37"/>
-      <c r="H122" s="160">
+      <c r="H122" s="151">
         <v>2.6328000000000001E-4</v>
       </c>
       <c r="I122" s="123" t="s">
@@ -7700,7 +7705,7 @@
       </c>
       <c r="F123" s="37"/>
       <c r="G123" s="37"/>
-      <c r="H123" s="160">
+      <c r="H123" s="151">
         <v>9.0165499999999996E-2</v>
       </c>
       <c r="I123" s="123" t="s">
@@ -7713,7 +7718,7 @@
       </c>
       <c r="F124" s="37"/>
       <c r="G124" s="37"/>
-      <c r="H124" s="160">
+      <c r="H124" s="151">
         <v>0</v>
       </c>
       <c r="I124" s="123" t="s">
@@ -7721,7 +7726,7 @@
       </c>
     </row>
     <row r="125" spans="5:9" customFormat="1" ht="16">
-      <c r="E125" s="159" t="s">
+      <c r="E125" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F125" s="37"/>
@@ -7734,13 +7739,13 @@
       </c>
     </row>
     <row r="126" spans="5:9" customFormat="1" ht="16">
-      <c r="E126" s="159"/>
+      <c r="E126" s="150"/>
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
       <c r="H126" s="23"/>
     </row>
     <row r="127" spans="5:9">
-      <c r="E127" s="149" t="s">
+      <c r="E127" s="140" t="s">
         <v>96</v>
       </c>
       <c r="F127" s="37"/>
@@ -7753,7 +7758,7 @@
       </c>
       <c r="F128" s="37"/>
       <c r="G128" s="37"/>
-      <c r="H128" s="160">
+      <c r="H128" s="151">
         <v>0</v>
       </c>
       <c r="I128" s="123" t="s">
@@ -7766,7 +7771,7 @@
       </c>
       <c r="F129" s="37"/>
       <c r="G129" s="37"/>
-      <c r="H129" s="160">
+      <c r="H129" s="151">
         <v>5.1643000000000001E-4</v>
       </c>
       <c r="I129" s="123" t="s">
@@ -7779,7 +7784,7 @@
       </c>
       <c r="F130" s="37"/>
       <c r="G130" s="37"/>
-      <c r="H130" s="160">
+      <c r="H130" s="151">
         <v>3.2445E-4</v>
       </c>
       <c r="I130" s="123" t="s">
@@ -7792,7 +7797,7 @@
       </c>
       <c r="F131" s="37"/>
       <c r="G131" s="37"/>
-      <c r="H131" s="160">
+      <c r="H131" s="151">
         <v>2.8475000000000001E-4</v>
       </c>
       <c r="I131" s="123" t="s">
@@ -7805,7 +7810,7 @@
       </c>
       <c r="F132" s="37"/>
       <c r="G132" s="37"/>
-      <c r="H132" s="160">
+      <c r="H132" s="151">
         <v>9.5493700000000001E-2</v>
       </c>
       <c r="I132" s="123" t="s">
@@ -7818,7 +7823,7 @@
       </c>
       <c r="F133" s="37"/>
       <c r="G133" s="37"/>
-      <c r="H133" s="160">
+      <c r="H133" s="151">
         <v>0</v>
       </c>
       <c r="I133" s="123" t="s">
@@ -7826,7 +7831,7 @@
       </c>
     </row>
     <row r="134" spans="5:9">
-      <c r="E134" s="159" t="s">
+      <c r="E134" s="150" t="s">
         <v>46</v>
       </c>
       <c r="F134" s="37"/>

</xml_diff>